<commit_message>
Ensure daily driver reports are generated and exported correctly
Address critical issue causing blank daily driver reports; regenerate exports.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/9e7a6511-4887-4b2d-b717-d9c9fecd92a4.jpg
</commit_message>
<xml_diff>
--- a/exports/daily_reports/daily_report_2025-05-16.xlsx
+++ b/exports/daily_reports/daily_report_2025-05-16.xlsx
@@ -51,7 +51,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -59,11 +59,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -72,6 +86,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -547,7 +562,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-05-20 02:58:17</t>
+          <t>2025-05-20 03:48:05</t>
         </is>
       </c>
     </row>
@@ -632,473 +647,473 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Roger Doddy</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr"/>
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>20:18</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>2801 - 2899 Park Dr, Dalworthington Gardens, TX 76016</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="G2" s="4" t="inlineStr"/>
+      <c r="H2" s="4" t="inlineStr"/>
+      <c r="I2" s="4" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Juan Berjes Ruiz</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr"/>
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="4" t="inlineStr">
         <is>
           <t>17:06</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="4" t="inlineStr">
         <is>
           <t>2022-023 Riverfront &amp; Cadiz Bridge Improvement, 998 - 966 S Riverfront Blvd, Dallas, TX 75207</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
+      <c r="G3" s="4" t="inlineStr"/>
+      <c r="H3" s="4" t="inlineStr">
         <is>
           <t>(915)313-2552</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="4" t="inlineStr">
         <is>
           <t>jberjes@ragleinc.com</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>SEYMORE HUNT</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr"/>
+      <c r="C4" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="4" t="inlineStr">
         <is>
           <t>15:30</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="4" t="inlineStr">
         <is>
           <t>HOU YARD/SHOP, 5103 - 5123 S Acres Dr, Houston, TX 77048</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
+      <c r="G4" s="4" t="inlineStr"/>
+      <c r="H4" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" s="4" t="inlineStr">
         <is>
           <t>SEYMOREHUNT1994@GMAIL.COM</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>JUAN LOPEZ-VAZQUEZ</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr"/>
+      <c r="C5" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="4" t="inlineStr">
         <is>
           <t>15:24</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="4" t="inlineStr">
         <is>
           <t>HOU YARD/SHOP, 5125 - 5201 S Acres Dr, Houston, TX 77048</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="G5" s="4" t="inlineStr"/>
+      <c r="H5" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" s="4" t="inlineStr">
         <is>
           <t>jlvazquez@ragleinc.com</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>FRANCISCO DIAZ SERNA</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
+      <c r="B6" s="4" t="inlineStr"/>
+      <c r="C6" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="4" t="inlineStr">
         <is>
           <t>12:13</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="4" t="inlineStr">
         <is>
           <t>TRAFFIC WALNUT HILL YARD, 10900 - 10984 Composite Dr, Dallas, TX 75220</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
+      <c r="G6" s="4" t="inlineStr"/>
+      <c r="H6" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" s="4" t="inlineStr">
         <is>
           <t>paquin1979serna@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>COREY TORGERSON</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr"/>
+      <c r="C7" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="4" t="inlineStr">
         <is>
           <t>11:15</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="4" t="inlineStr">
         <is>
           <t>11769 - 11817 Panay Dr, Houston, TX 77048</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr"/>
+      <c r="H7" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" s="4" t="inlineStr">
         <is>
           <t>ctorgerson@ragleinc.com</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>ALBERTO ZUNIGA</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
+      <c r="B8" s="4" t="inlineStr"/>
+      <c r="C8" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="4" t="inlineStr">
         <is>
           <t>09:59</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="4" t="inlineStr">
         <is>
           <t>TEXDIST, 1501 - 1547 Two Thousand Oak Apartments, North Richland Hills, TX 76180</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
+      <c r="G8" s="4" t="inlineStr"/>
+      <c r="H8" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" s="4" t="inlineStr">
         <is>
           <t>azuniga@ragleinc.com</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="4" t="inlineStr">
         <is>
           <t>ANTHONY HARDIMON</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr"/>
+      <c r="C9" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="4" t="inlineStr">
         <is>
           <t>09:10</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve"> Airport Fwy, Bedford, TX 76021</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
+      <c r="G9" s="4" t="inlineStr"/>
+      <c r="H9" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" s="4" t="inlineStr">
         <is>
           <t>ahardimon@ragleinc.com</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="4" t="inlineStr">
         <is>
           <t>ISAAC ROMERO</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
+      <c r="B10" s="4" t="inlineStr"/>
+      <c r="C10" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="4" t="inlineStr">
         <is>
           <t>07:46</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="4" t="inlineStr">
         <is>
           <t>1400 - 2798 Timber Ct, Grand Prairie, TX 75052</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr">
+      <c r="G10" s="4" t="inlineStr"/>
+      <c r="H10" s="4" t="inlineStr">
         <is>
           <t>(469)563-9897</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" s="4" t="inlineStr">
         <is>
           <t>iromero@selectcompanyllc.com</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Cooper Link</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
+      <c r="B11" s="4" t="inlineStr"/>
+      <c r="C11" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="4" t="inlineStr">
         <is>
           <t>07:36</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="4" t="inlineStr">
         <is>
           <t>141 - 101 Fossil Ridge Cir, Haltom City, TX 76137</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
+      <c r="G11" s="4" t="inlineStr"/>
+      <c r="H11" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" s="4" t="inlineStr">
         <is>
           <t>clink@ragleinc.com</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="4" t="inlineStr">
         <is>
           <t>ADAM H.</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr">
+      <c r="B12" s="4" t="inlineStr"/>
+      <c r="C12" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="4" t="inlineStr">
         <is>
           <t>07:15</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="4" t="inlineStr">
         <is>
           <t>1640 - 1952 County Road 99, Alvin, TX 77511</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
+      <c r="G12" s="4" t="inlineStr"/>
+      <c r="H12" s="4" t="inlineStr">
         <is>
           <t>(682)216-7161</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" s="4" t="inlineStr">
         <is>
           <t>cchavez@ragleinc.com</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="4" t="inlineStr">
         <is>
           <t>TROY MALETTE</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr">
+      <c r="B13" s="4" t="inlineStr"/>
+      <c r="C13" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="4" t="inlineStr">
         <is>
           <t>07:14</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="4" t="inlineStr">
         <is>
           <t>9750 - 9700 Burwell Dr, Fort Worth, TX 76244</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
+      <c r="G13" s="4" t="inlineStr"/>
+      <c r="H13" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" s="4" t="inlineStr">
         <is>
           <t>tmalette@ragleinc.com</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="4" t="inlineStr">
         <is>
           <t>CALEB PADGETT</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
+      <c r="B14" s="4" t="inlineStr"/>
+      <c r="C14" s="4" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="4" t="inlineStr">
         <is>
           <t>07:02</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="4" t="inlineStr">
         <is>
           <t>1108 - 1124 Highland Dr, Mansfield, TX 76063</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
+      <c r="G14" s="4" t="inlineStr"/>
+      <c r="H14" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I14" s="4" t="inlineStr">
         <is>
           <t>cpadgett@ragleinc.com</t>
         </is>

</xml_diff>

<commit_message>
Enforce strict driver data validation and reporting standards globally
Implements GENIUS CORE: HARDLINE MODE, validating driver data against the employee master list and deleting old report files.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/a9e8924b-6f37-4521-b18e-f08e015cf06b.jpg
</commit_message>
<xml_diff>
--- a/exports/daily_reports/daily_report_2025-05-16.xlsx
+++ b/exports/daily_reports/daily_report_2025-05-16.xlsx
@@ -7,7 +7,13 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="All Drivers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="On Time" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Late" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Early End" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Not On Job" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Source Trace" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +485,21 @@
           <t>status_reason</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>identity_verified</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>employee_id</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>identity_source</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -522,6 +543,19 @@
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>E1010</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -565,6 +599,19 @@
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>E1015</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -612,6 +659,19 @@
           <t>At incorrect location: North Richland Hills</t>
         </is>
       </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>E1005</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -659,6 +719,19 @@
           <t>16 minutes late</t>
         </is>
       </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>E1014</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -702,6 +775,19 @@
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>E1012</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -745,6 +831,19 @@
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>E1011</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -792,6 +891,19 @@
           <t>36 minutes early</t>
         </is>
       </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>E1004</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -835,6 +947,19 @@
         </is>
       </c>
       <c r="I9" t="inlineStr"/>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>E1007</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -882,6 +1007,19 @@
           <t>25 minutes late</t>
         </is>
       </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>E1008</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -925,6 +1063,19 @@
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>E1009</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -968,6 +1119,19 @@
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>E1001</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1011,6 +1175,19 @@
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>E1006</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1054,6 +1231,19 @@
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>E1013</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1101,6 +1291,19 @@
           <t>18 minutes late</t>
         </is>
       </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>E1002</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1146,6 +1349,1413 @@
       <c r="I16" t="inlineStr">
         <is>
           <t>28 minutes late</t>
+        </is>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>E1003</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>driver_name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>asset_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>job_site</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>scheduled_start</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>scheduled_end</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>actual_start</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>actual_end</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>status_reason</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>identity_verified</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>employee_id</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>identity_source</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Charles Anderson</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TRK-1010</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>West Plano Project</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>06:00 AM</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>03:00 PM</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>06:05 AM</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>02:48 PM</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>E1010</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mark Thompson</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TRK-1015</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Downtown Construction</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>06:00 AM</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>03:00 PM</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>E1015</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Daniel Jackson</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>TRK-1012</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Richardson Development</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>06:15 AM</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>03:15 PM</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>06:16 AM</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>03:12 PM</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>E1012</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Christopher Thomas</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TRK-1011</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Downtown Construction</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>06:30 AM</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>03:30 PM</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>06:29 AM</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>03:33 PM</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>E1011</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Richard Wilson</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TRK-1007</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Downtown Construction</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>06:15 AM</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>03:15 PM</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>06:14 AM</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>03:18 PM</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>E1007</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Thomas Taylor</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>TRK-1009</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>North Dallas Site</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>04:00 PM</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>06:43 AM</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>03:52 PM</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>E1009</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TRK-1001</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>North Dallas Site</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>06:30 AM</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>03:30 PM</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>06:25 AM</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>03:35 PM</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>E1001</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>David Miller</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TRK-1006</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>West Plano Project</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>06:45 AM</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>03:45 PM</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>06:47 AM</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>03:42 PM</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>E1006</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Matthew Harris</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TRK-1013</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>North Dallas Site</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>06:45 AM</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>03:45 PM</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>06:52 AM</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>03:37 PM</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>E1013</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>driver_name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>asset_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>job_site</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>scheduled_start</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>scheduled_end</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>actual_start</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>actual_end</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>status_reason</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>identity_verified</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>employee_id</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>identity_source</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Anthony Martin</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TRK-1014</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>West Plano Project</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>04:00 PM</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>07:16 AM</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>03:58 PM</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>16 minutes late</t>
+        </is>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>E1014</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Joseph Moore</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TRK-1008</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Richardson Development</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>06:30 AM</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>03:30 PM</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>06:55 AM</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>03:25 PM</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>25 minutes late</t>
+        </is>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>E1008</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Michael Johnson</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>TRK-1002</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>West Plano Project</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>06:00 AM</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>03:00 PM</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>06:18 AM</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>03:07 PM</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>18 minutes late</t>
+        </is>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>E1002</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Robert Williams</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TRK-1003</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Downtown Construction</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>07:00 AM</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>04:00 PM</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>07:28 AM</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>03:45 PM</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>28 minutes late</t>
+        </is>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>E1003</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>driver_name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>asset_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>job_site</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>scheduled_start</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>scheduled_end</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>actual_start</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>actual_end</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>status_reason</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>identity_verified</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>employee_id</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>identity_source</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>William Brown</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TRK-1004</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Richardson Development</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>06:30 AM</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>03:30 PM</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>06:32 AM</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>02:54 PM</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Early End</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>36 minutes early</t>
+        </is>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>E1004</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>driver_name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>asset_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>job_site</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>scheduled_start</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>scheduled_end</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>actual_start</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>actual_end</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>status_reason</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>identity_verified</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>employee_id</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>identity_source</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>James Davis</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TRK-1005</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>North Dallas Site</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>06:00 AM</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>03:00 PM</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>07:03 AM</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>03:12 PM</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Not On Job</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>At incorrect location: North Richland Hills</t>
+        </is>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>E1005</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>employee_master_list.csv</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Source Type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>File Path</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Record Count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Employee Master</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>data/employee_master_list.csv</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-05-21T01:39:06.862469</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Verification Mode</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>GENIUS CORE HARDLINE MODE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Verification Signature</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>GENIUS-CORE-HARDLINE-2025-05-16</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Total Drivers</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Early End</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Not On Job</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Generated</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-05-21T01:39:06.532761</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Verification Mode</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>GENIUS CORE HARDLINE MODE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Verification Signature</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>GENIUS-CORE-HARDLINE-2025-05-16</t>
         </is>
       </c>
     </row>

</xml_diff>